<commit_message>
#940 Regenerated template definition and xlsx files
</commit_message>
<xml_diff>
--- a/backend/excel_templates/findings-uniform-guidance-template.xlsx
+++ b/backend/excel_templates/findings-uniform-guidance-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="108FAD3997BE6" lockStructure="1"/>
+  <workbookProtection workbookPassword="10C841849C163" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -51497,7 +51497,7 @@
       <c r="O2999" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="108FAD3997BE6"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="10C841849C163"/>
   <mergeCells count="2">
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="C2:O2"/>

</xml_diff>